<commit_message>
Update gantt chart to have project 3
</commit_message>
<xml_diff>
--- a/studytracker/Gant.xlsx
+++ b/studytracker/Gant.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Actual">(PeriodInActual*(project!$G1&gt;0))*PeriodInPlan</definedName>
-    <definedName name="ActualBeyond">PeriodInActual*(project!$G1&gt;0)</definedName>
+    <definedName name="Actual">(PeriodInActual*(project!$I1&gt;0))*PeriodInPlan</definedName>
+    <definedName name="ActualBeyond">PeriodInActual*(project!$I1&gt;0)</definedName>
     <definedName name="PercentComplete">PercentCompleteBeyond*PeriodInPlan</definedName>
-    <definedName name="PercentCompleteBeyond">(project!A$8=MEDIAN(project!A$8,project!$G1,project!$G1+project!$H1)*(project!$G1&gt;0))*((project!A$8&lt;(INT(project!$G1+project!$H1*project!$I1)))+(project!A$8=project!$G1))*(project!$I1&gt;0)</definedName>
-    <definedName name="period_selected">project!$P$3</definedName>
-    <definedName name="PeriodInActual">project!A$8=MEDIAN(project!A$8,project!$G1,project!$G1+project!$H1-1)</definedName>
+    <definedName name="PercentCompleteBeyond">(project!A$8=MEDIAN(project!A$8,project!$I1,project!$I1+project!$J1)*(project!$I1&gt;0))*((project!A$8&lt;(INT(project!$I1+project!$J1*project!$K1)))+(project!A$8=project!$I1))*(project!$K1&gt;0)</definedName>
+    <definedName name="period_selected">project!$R$3</definedName>
+    <definedName name="PeriodInActual">project!A$8=MEDIAN(project!A$8,project!$I1,project!$I1+project!$J1-1)</definedName>
     <definedName name="PeriodInPlan">project!A$8=MEDIAN(project!A$8,project!$E1,project!$E1+project!$F1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*(project!$E1&gt;0)</definedName>
   </definedNames>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
   <si>
     <t>Project Planner</t>
   </si>
@@ -288,6 +288,18 @@
   </si>
   <si>
     <t>browser bot</t>
+  </si>
+  <si>
+    <t>Optimistic</t>
+  </si>
+  <si>
+    <t>Realistic</t>
+  </si>
+  <si>
+    <t>Pessimistic</t>
+  </si>
+  <si>
+    <t>Create productivity graphs</t>
   </si>
 </sst>
 </file>
@@ -791,13 +803,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>16</xdr:col>
+          <xdr:col>18</xdr:col>
           <xdr:colOff>66675</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>16</xdr:col>
+          <xdr:col>18</xdr:col>
           <xdr:colOff>200025</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>257175</xdr:rowOff>
@@ -1067,10 +1079,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BS35"/>
+  <dimension ref="B1:BU36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1081,102 +1093,110 @@
     <col min="4" max="4" width="9.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.25" style="18" customWidth="1"/>
     <col min="6" max="6" width="7.25" style="23" customWidth="1"/>
-    <col min="7" max="7" width="7.25" style="18" customWidth="1"/>
-    <col min="8" max="8" width="8.375" style="18" customWidth="1"/>
-    <col min="9" max="10" width="7.25" style="6" customWidth="1"/>
-    <col min="11" max="15" width="7.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="7.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="30" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="41" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="50" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="51" max="70" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.25" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.25" style="18" customWidth="1"/>
+    <col min="10" max="10" width="8.375" style="18" customWidth="1"/>
+    <col min="11" max="12" width="7.25" style="6" customWidth="1"/>
+    <col min="13" max="17" width="7.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="7.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="32" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="43" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="52" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="53" max="72" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:71" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:73" x14ac:dyDescent="0.3">
       <c r="E1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="2:71" ht="54" x14ac:dyDescent="0.8">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="2:73" ht="54" x14ac:dyDescent="0.8">
       <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="24"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="2:71" ht="21" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="2:73" ht="21" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="24"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
-      <c r="P3" s="22">
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="22">
         <f ca="1">NOW()</f>
-        <v>42471.735437962961</v>
-      </c>
-      <c r="Q3" s="7"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="14" t="s">
+        <v>42474.402628124997</v>
+      </c>
+      <c r="S3" s="7"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="V3" s="9"/>
-      <c r="W3" s="14" t="s">
+      <c r="X3" s="9"/>
+      <c r="Y3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="5" t="s">
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="5" t="s">
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="5" t="s">
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="12"/>
+      <c r="AP3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:71" ht="18.75" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="4" spans="2:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="24"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
-      <c r="AV4" s="1"/>
-      <c r="AW4" s="1"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
       <c r="AX4" s="1"/>
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
-    </row>
-    <row r="5" spans="2:71" x14ac:dyDescent="0.3">
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="1"/>
+    </row>
+    <row r="5" spans="2:73" x14ac:dyDescent="0.3">
       <c r="E5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="AV5" s="1"/>
-      <c r="AW5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
       <c r="AX5" s="1"/>
-    </row>
-    <row r="6" spans="2:71" ht="15" x14ac:dyDescent="0.25">
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+    </row>
+    <row r="6" spans="2:73" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1184,27 +1204,33 @@
         <v>3</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="AV6" s="1"/>
-      <c r="AW6" s="1"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
       <c r="AX6" s="1"/>
-    </row>
-    <row r="7" spans="2:71" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+    </row>
+    <row r="7" spans="2:73" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1218,173 +1244,179 @@
       <c r="F7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="2:71" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="2:73" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="26"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
-      <c r="K8" s="17">
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17">
         <v>42452</v>
       </c>
-      <c r="L8" s="17">
+      <c r="N8" s="17">
         <v>42453</v>
       </c>
-      <c r="M8" s="17">
+      <c r="O8" s="17">
         <v>42454</v>
       </c>
-      <c r="N8" s="17">
+      <c r="P8" s="17">
         <v>42455</v>
       </c>
-      <c r="O8" s="17">
+      <c r="Q8" s="17">
         <v>42456</v>
       </c>
-      <c r="P8" s="17">
+      <c r="R8" s="17">
         <v>42457</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="S8" s="17">
         <v>42458</v>
       </c>
-      <c r="R8" s="17">
+      <c r="T8" s="17">
         <v>42459</v>
       </c>
-      <c r="S8" s="17">
+      <c r="U8" s="17">
         <v>42460</v>
       </c>
-      <c r="T8" s="17">
+      <c r="V8" s="17">
         <v>42461</v>
       </c>
-      <c r="U8" s="17">
+      <c r="W8" s="17">
         <v>42462</v>
       </c>
-      <c r="V8" s="17">
+      <c r="X8" s="17">
         <v>42463</v>
       </c>
-      <c r="W8" s="17">
+      <c r="Y8" s="17">
         <v>42464</v>
       </c>
-      <c r="X8" s="17">
+      <c r="Z8" s="17">
         <v>42465</v>
       </c>
-      <c r="Y8" s="17">
+      <c r="AA8" s="17">
         <v>42466</v>
       </c>
-      <c r="Z8" s="17">
+      <c r="AB8" s="17">
         <v>42467</v>
       </c>
-      <c r="AA8" s="17">
+      <c r="AC8" s="17">
         <v>42468</v>
       </c>
-      <c r="AB8" s="17">
+      <c r="AD8" s="17">
         <v>42469</v>
       </c>
-      <c r="AC8" s="17">
+      <c r="AE8" s="17">
         <v>42470</v>
       </c>
-      <c r="AD8" s="17">
+      <c r="AF8" s="17">
         <v>42471</v>
       </c>
-      <c r="AE8" s="17">
+      <c r="AG8" s="17">
         <v>42472</v>
       </c>
-      <c r="AF8" s="17">
+      <c r="AH8" s="17">
         <v>42473</v>
       </c>
-      <c r="AG8" s="17">
+      <c r="AI8" s="17">
         <v>42474</v>
       </c>
-      <c r="AH8" s="17">
+      <c r="AJ8" s="17">
         <v>42475</v>
       </c>
-      <c r="AI8" s="17">
+      <c r="AK8" s="17">
         <v>42476</v>
       </c>
-      <c r="AJ8" s="17">
+      <c r="AL8" s="17">
         <v>42477</v>
       </c>
-      <c r="AK8" s="17">
+      <c r="AM8" s="17">
         <v>42478</v>
       </c>
-      <c r="AL8" s="17">
+      <c r="AN8" s="17">
         <v>42479</v>
       </c>
-      <c r="AM8" s="17">
+      <c r="AO8" s="17">
         <v>42480</v>
       </c>
-      <c r="AN8" s="17">
+      <c r="AP8" s="17">
         <v>42481</v>
       </c>
-      <c r="AO8" s="17">
+      <c r="AQ8" s="17">
         <v>42482</v>
       </c>
-      <c r="AP8" s="17">
+      <c r="AR8" s="17">
         <v>42483</v>
       </c>
-      <c r="AQ8" s="17">
+      <c r="AS8" s="17">
         <v>42484</v>
       </c>
-      <c r="AR8" s="17">
+      <c r="AT8" s="17">
         <v>42485</v>
       </c>
-      <c r="AS8" s="17">
+      <c r="AU8" s="17">
         <v>42486</v>
       </c>
-      <c r="AT8" s="17">
+      <c r="AV8" s="17">
         <v>42487</v>
       </c>
-      <c r="AU8" s="17">
+      <c r="AW8" s="17">
         <v>42488</v>
       </c>
-      <c r="AV8" s="17">
+      <c r="AX8" s="17">
         <v>42489</v>
       </c>
-      <c r="AW8" s="17">
+      <c r="AY8" s="17">
         <v>42490</v>
       </c>
-      <c r="AX8" s="17">
+      <c r="AZ8" s="17">
         <v>42491</v>
       </c>
-      <c r="AY8" s="17">
+      <c r="BA8" s="17">
         <v>42492</v>
       </c>
-      <c r="AZ8" s="17">
+      <c r="BB8" s="17">
         <v>42493</v>
       </c>
-      <c r="BA8" s="17">
+      <c r="BC8" s="17">
         <v>42494</v>
       </c>
-      <c r="BB8" s="17">
+      <c r="BD8" s="17">
         <v>42495</v>
       </c>
-      <c r="BC8" s="17">
+      <c r="BE8" s="17">
         <v>42496</v>
       </c>
-      <c r="BD8" s="17">
+      <c r="BF8" s="17">
         <v>42497</v>
       </c>
-      <c r="BE8" s="17"/>
-      <c r="BF8" s="17"/>
       <c r="BG8" s="17"/>
       <c r="BH8" s="17"/>
       <c r="BI8" s="17"/>
@@ -1397,11 +1429,13 @@
       <c r="BP8" s="17"/>
       <c r="BQ8" s="17"/>
       <c r="BR8" s="17"/>
-      <c r="BS8" s="18"/>
-    </row>
-    <row r="9" spans="2:71" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
-        <v>40</v>
+      <c r="BS8" s="17"/>
+      <c r="BT8" s="17"/>
+      <c r="BU8" s="18"/>
+    </row>
+    <row r="9" spans="2:73" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="20">
         <v>42452</v>
@@ -1409,411 +1443,532 @@
       <c r="F9" s="27">
         <v>1</v>
       </c>
-      <c r="G9" s="20">
-        <v>42463</v>
+      <c r="G9" s="27">
+        <v>3</v>
       </c>
       <c r="H9" s="27">
-        <v>2</v>
-      </c>
-      <c r="I9" s="13">
-        <v>0</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:71" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
-        <v>41</v>
+        <v>5</v>
+      </c>
+      <c r="I9" s="20">
+        <v>42454</v>
+      </c>
+      <c r="J9" s="27">
+        <v>3</v>
+      </c>
+      <c r="K9" s="13">
+        <v>1</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:73" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>29</v>
       </c>
       <c r="E10" s="20">
-        <v>42471</v>
+        <v>42452</v>
       </c>
       <c r="F10" s="27">
-        <v>7</v>
-      </c>
-      <c r="G10" s="20">
-        <v>42471</v>
+        <v>1</v>
+      </c>
+      <c r="G10" s="27">
+        <v>3</v>
       </c>
       <c r="H10" s="27">
-        <v>0</v>
-      </c>
-      <c r="I10" s="13">
-        <v>0</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:71" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="I10" s="20">
+        <v>42454</v>
+      </c>
+      <c r="J10" s="27">
+        <v>3</v>
+      </c>
+      <c r="K10" s="13">
+        <v>1</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:73" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E11" s="20">
-        <v>42463</v>
+        <v>42456</v>
       </c>
       <c r="F11" s="27">
         <v>1</v>
       </c>
-      <c r="G11" s="20">
-        <v>42465</v>
+      <c r="G11" s="27">
+        <v>3</v>
       </c>
       <c r="H11" s="27">
-        <v>0</v>
-      </c>
-      <c r="I11" s="13">
-        <v>0</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:71" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
-        <v>46</v>
+        <v>5</v>
+      </c>
+      <c r="I11" s="20">
+        <v>42462</v>
+      </c>
+      <c r="J11" s="27">
+        <v>1</v>
+      </c>
+      <c r="K11" s="13">
+        <v>1</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:73" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
+        <v>31</v>
       </c>
       <c r="E12" s="20">
-        <v>42464</v>
+        <v>42456</v>
       </c>
       <c r="F12" s="27">
         <v>1</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="27">
+        <v>3</v>
+      </c>
+      <c r="H12" s="27">
+        <v>5</v>
+      </c>
+      <c r="I12" s="20">
+        <v>42462</v>
+      </c>
+      <c r="J12" s="27">
+        <v>1</v>
+      </c>
+      <c r="K12" s="13">
+        <v>1</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:73" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="20">
+        <v>42456</v>
+      </c>
+      <c r="F13" s="27">
+        <v>2</v>
+      </c>
+      <c r="G13" s="27">
+        <v>3</v>
+      </c>
+      <c r="H13" s="27">
+        <v>6</v>
+      </c>
+      <c r="I13" s="20">
         <v>42464</v>
       </c>
-      <c r="H12" s="27">
-        <v>0</v>
-      </c>
-      <c r="I12" s="13">
-        <v>0</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="2:71" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="20">
-        <v>42465</v>
-      </c>
-      <c r="F13" s="27">
+      <c r="J13" s="27">
+        <v>2</v>
+      </c>
+      <c r="K13" s="13">
         <v>1</v>
       </c>
-      <c r="G13" s="20">
-        <v>42465</v>
-      </c>
-      <c r="H13" s="27">
-        <v>0</v>
-      </c>
-      <c r="I13" s="13">
-        <v>0</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:71" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:73" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="29" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E14" s="20">
-        <v>42466</v>
+        <v>42454</v>
       </c>
       <c r="F14" s="27">
         <v>1</v>
       </c>
-      <c r="G14" s="20">
-        <v>42466</v>
+      <c r="G14" s="27">
+        <v>3</v>
       </c>
       <c r="H14" s="27">
-        <v>0</v>
-      </c>
-      <c r="I14" s="13">
-        <v>0</v>
-      </c>
-      <c r="J14" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="20">
+        <v>42458</v>
+      </c>
+      <c r="J14" s="27">
+        <v>6</v>
+      </c>
+      <c r="K14" s="13">
+        <v>1</v>
+      </c>
+      <c r="L14" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:71" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:73" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="29" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E15" s="20">
-        <v>42467</v>
+        <v>42454</v>
       </c>
       <c r="F15" s="27">
+        <v>2</v>
+      </c>
+      <c r="G15" s="27">
+        <v>4</v>
+      </c>
+      <c r="H15" s="27">
+        <v>6</v>
+      </c>
+      <c r="I15" s="20">
+        <v>42458</v>
+      </c>
+      <c r="J15" s="27">
+        <v>4</v>
+      </c>
+      <c r="K15" s="13">
         <v>1</v>
       </c>
-      <c r="G15" s="20">
-        <v>42467</v>
-      </c>
-      <c r="H15" s="27">
-        <v>0</v>
-      </c>
-      <c r="I15" s="13">
-        <v>0</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:71" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:73" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="E16" s="20">
-        <v>42468</v>
+        <v>42459</v>
       </c>
       <c r="F16" s="27">
         <v>1</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="27">
+        <v>3</v>
+      </c>
+      <c r="H16" s="27">
+        <v>5</v>
+      </c>
+      <c r="I16" s="20">
+        <v>42463</v>
+      </c>
+      <c r="J16" s="27">
+        <v>4</v>
+      </c>
+      <c r="K16" s="13">
+        <v>1</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="20">
         <v>42468</v>
-      </c>
-      <c r="H16" s="27">
-        <v>0</v>
-      </c>
-      <c r="I16" s="13">
-        <v>0</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="20">
-        <v>42469</v>
       </c>
       <c r="F17" s="27">
         <v>1</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="20">
+        <v>42468</v>
+      </c>
+      <c r="J17" s="27">
+        <v>0</v>
+      </c>
+      <c r="K17" s="13">
+        <v>0</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="20">
         <v>42469</v>
-      </c>
-      <c r="H17" s="27">
-        <v>0</v>
-      </c>
-      <c r="I17" s="13">
-        <v>0</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="20">
-        <v>42470</v>
       </c>
       <c r="F18" s="27">
         <v>1</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="20">
+        <v>42469</v>
+      </c>
+      <c r="J18" s="27">
+        <v>0</v>
+      </c>
+      <c r="K18" s="13">
+        <v>0</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="20">
         <v>42470</v>
-      </c>
-      <c r="H18" s="27">
-        <v>0</v>
-      </c>
-      <c r="I18" s="13">
-        <v>0</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="20">
-        <v>42471</v>
       </c>
       <c r="F19" s="27">
         <v>1</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="20">
+        <v>42470</v>
+      </c>
+      <c r="J19" s="27">
+        <v>0</v>
+      </c>
+      <c r="K19" s="13">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="20">
         <v>42471</v>
       </c>
-      <c r="H19" s="27">
+      <c r="F20" s="27">
+        <v>1</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="20">
+        <v>42471</v>
+      </c>
+      <c r="J20" s="27">
         <v>0</v>
       </c>
-      <c r="I19" s="13">
+      <c r="K20" s="13">
         <v>0</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="L20" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="27">
-        <v>2</v>
-      </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="29" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="27"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="27">
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="27">
         <v>2</v>
       </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13" t="s">
+      <c r="K21" s="13"/>
+      <c r="L21" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="29" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="27"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="27">
+        <v>2</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="29" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="27"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-    </row>
-    <row r="24" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="29"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>42</v>
+      </c>
       <c r="E25" s="20"/>
       <c r="F25" s="27"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-    </row>
-    <row r="26" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="29"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="E26" s="20"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-    </row>
-    <row r="27" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="29"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+    </row>
+    <row r="27" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="E27" s="20"/>
       <c r="F27" s="27"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-    </row>
-    <row r="28" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="29"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
+        <v>57</v>
+      </c>
       <c r="E28" s="20"/>
       <c r="F28" s="27"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-    </row>
-    <row r="29" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="29"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="29" t="s">
+        <v>58</v>
+      </c>
       <c r="E29" s="20"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-    </row>
-    <row r="30" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="29"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+    </row>
+    <row r="30" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="E30" s="20"/>
       <c r="F30" s="27"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-    </row>
-    <row r="31" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="29"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="29" t="s">
+        <v>61</v>
+      </c>
       <c r="E31" s="20"/>
       <c r="F31" s="27"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+    </row>
+    <row r="32" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="29"/>
       <c r="E32" s="20"/>
       <c r="F32" s="27"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-    </row>
-    <row r="33" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+    </row>
+    <row r="33" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="29"/>
       <c r="E33" s="20"/>
       <c r="F33" s="27"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-    </row>
-    <row r="34" spans="2:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+    </row>
+    <row r="34" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="29"/>
       <c r="E34" s="20"/>
       <c r="F34" s="27"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+    </row>
+    <row r="35" spans="2:12" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="29"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="29"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K9:BR34">
+  <conditionalFormatting sqref="M9:BT35">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1830,7 +1985,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="7">
-      <formula>K$8=period_selected</formula>
+      <formula>M$8=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
@@ -1839,31 +1994,31 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:BR35">
+  <conditionalFormatting sqref="B36:BT36">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BR8">
+  <conditionalFormatting sqref="M8:BT8">
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>K$8=period_selected</formula>
+      <formula>M$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3">
       <formula1>42461</formula1>
       <formula2>42496</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:XFD8 E9:E1048576 A8:E8 G8:G1048576">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:XFD8 E9:E1048576 A8:E8 I8:I1048576">
       <formula1>42452</formula1>
       <formula2>42496</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576 H1:H1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576 F1:H5 F7:H1048576">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:D1048576">
-      <formula1>$B$9:$B$1048576</formula1>
+      <formula1>$B$15:$B$1048576</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -1879,13 +2034,13 @@
               <controlPr defaultSize="0" print="0" autoPict="0" altText="Period Highlight Spin Control">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>16</xdr:col>
+                    <xdr:col>18</xdr:col>
                     <xdr:colOff>66675</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>16</xdr:col>
+                    <xdr:col>18</xdr:col>
                     <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>257175</xdr:rowOff>
@@ -1900,18 +2055,24 @@
   </mc:AlternateContent>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:J7 J9:J1048576</xm:sqref>
+          <xm:sqref>L1:L7 L9:L14 L17:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet1!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I1:I7 I9:I1048576</xm:sqref>
+          <xm:sqref>K1:K7 K9:K1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet1!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>L15:L16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1926,8 +2087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor change, update Gant chart progress
</commit_message>
<xml_diff>
--- a/studytracker/Gant.xlsx
+++ b/studytracker/Gant.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
@@ -20,8 +20,7 @@
     <definedName name="PeriodInPlan">project!A$8=MEDIAN(project!A$8,project!$E1,project!$E1+project!$F1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*(project!$E1&gt;0)</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -325,7 +324,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
@@ -1101,8 +1100,8 @@
   </sheetPr>
   <dimension ref="B1:BU38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1163,7 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="22">
         <f ca="1">NOW()</f>
-        <v>42474.556638657406</v>
+        <v>42499.524256712961</v>
       </c>
       <c r="S3" s="7"/>
       <c r="U3" s="8"/>
@@ -1729,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="13" t="s">
         <v>18</v>
@@ -1783,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="13">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L20" s="13" t="s">
         <v>18</v>
@@ -2021,7 +2020,9 @@
       </c>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="13">
+        <v>0.5</v>
+      </c>
       <c r="L31" s="13" t="s">
         <v>18</v>
       </c>

</xml_diff>